<commit_message>
add: fill mode for restricted exam; incomplete (no xlsx export yet)
</commit_message>
<xml_diff>
--- a/manual/sample_with_image.xlsx
+++ b/manual/sample_with_image.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\exam_builder\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C0EA1C-8FC4-45B2-9B33-63FD2D9F8947}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AC038F-386D-4D5C-9E8B-20171943FDF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="152">
   <si>
     <t>question</t>
   </si>
@@ -408,9 +408,6 @@
     <t>Coaxial machine gun</t>
   </si>
   <si>
-    <t>650hp engine</t>
-  </si>
-  <si>
     <t>The AM upgrade of the T-55 added to its turret armor:</t>
   </si>
   <si>
@@ -469,6 +466,21 @@
   </si>
   <si>
     <t>Increased smoke evacuation</t>
+  </si>
+  <si>
+    <t>Which ERA cannot degrade solid penetrator e.g APFSDS?</t>
+  </si>
+  <si>
+    <t>Kontakt-1</t>
+  </si>
+  <si>
+    <t>Kontakt-5</t>
+  </si>
+  <si>
+    <t>All of them can</t>
+  </si>
+  <si>
+    <t>581hp engine</t>
   </si>
 </sst>
 </file>
@@ -1643,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ30"/>
+  <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2285,7 @@
         <v>126</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
@@ -2281,19 +2293,19 @@
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="F27" s="1">
         <v>4</v>
@@ -2301,19 +2313,19 @@
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
@@ -2321,19 +2333,19 @@
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="F29" s="1">
         <v>2</v>
@@ -2341,25 +2353,45 @@
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>102</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: switching to billboardjs, still not working
</commit_message>
<xml_diff>
--- a/manual/sample_with_image.xlsx
+++ b/manual/sample_with_image.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\exam_builder\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AC038F-386D-4D5C-9E8B-20171943FDF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686897A-8A95-4DB9-A502-09E1640DF7EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="269">
   <si>
     <t>question</t>
   </si>
@@ -267,9 +267,6 @@
     <t>T-80BVM</t>
   </si>
   <si>
-    <t>Which of the following vehicle is not a BMP?</t>
-  </si>
-  <si>
     <t>The 2K22 Tunguska was designed to replace the ZSU-23-4 Shilka due to</t>
   </si>
   <si>
@@ -481,6 +478,360 @@
   </si>
   <si>
     <t>581hp engine</t>
+  </si>
+  <si>
+    <t>Which of the following helicopter can transport troops by default?</t>
+  </si>
+  <si>
+    <t>Mi-24</t>
+  </si>
+  <si>
+    <t>Ka-52</t>
+  </si>
+  <si>
+    <t>Ka-50</t>
+  </si>
+  <si>
+    <t>Mi-28</t>
+  </si>
+  <si>
+    <t>How many missiles can a Mi-24V carries?</t>
+  </si>
+  <si>
+    <t>Which of the following vehicle does not belong to the BMP family?</t>
+  </si>
+  <si>
+    <t>Fly-by-wire control system</t>
+  </si>
+  <si>
+    <t>Canard wings, reducing distance needed before liftoff</t>
+  </si>
+  <si>
+    <t>Vympel R-73 short range air-to-air missles</t>
+  </si>
+  <si>
+    <t>Zaslon heavy radar with detection range up to 200km</t>
+  </si>
+  <si>
+    <t>The original name of the project that created the Su-27 and Mig-29 is</t>
+  </si>
+  <si>
+    <t>PFI (ПФИ)</t>
+  </si>
+  <si>
+    <t>TPFI (ТПФИ)</t>
+  </si>
+  <si>
+    <t>LPFI (ЛПФИ)</t>
+  </si>
+  <si>
+    <t>RPFI (РПФИ)</t>
+  </si>
+  <si>
+    <t>After the N-019 pulse-doppler radar complex was leaked to the West, the Soviet created a modified variant which is</t>
+  </si>
+  <si>
+    <t>N-019M Topaz</t>
+  </si>
+  <si>
+    <t>N-010 Zhuk-M</t>
+  </si>
+  <si>
+    <t>N-010A Zhuk-MA/MAE</t>
+  </si>
+  <si>
+    <t>No such variant exist</t>
+  </si>
+  <si>
+    <t>image_1</t>
+  </si>
+  <si>
+    <t>image_2</t>
+  </si>
+  <si>
+    <t>image_3</t>
+  </si>
+  <si>
+    <t>image_4</t>
+  </si>
+  <si>
+    <t>image_5</t>
+  </si>
+  <si>
+    <t>image_6</t>
+  </si>
+  <si>
+    <t>Which of the following plane is a MiG-23?</t>
+  </si>
+  <si>
+    <t>Which update of the M1 Abrams gave it a 120mm gun?</t>
+  </si>
+  <si>
+    <t>M1A1</t>
+  </si>
+  <si>
+    <t>M1IP</t>
+  </si>
+  <si>
+    <t>M1A2</t>
+  </si>
+  <si>
+    <t>M1A1HA</t>
+  </si>
+  <si>
+    <t>M1A1HC</t>
+  </si>
+  <si>
+    <t>The first upgrade to give the M1 Abrams depleted uranium armor is:</t>
+  </si>
+  <si>
+    <t>An additional machine gun</t>
+  </si>
+  <si>
+    <t>The SEP package for the M1A2 gives it:</t>
+  </si>
+  <si>
+    <t>Upgraded third-generation depleted uranium armor</t>
+  </si>
+  <si>
+    <t>Second-generation gunner thermal sight</t>
+  </si>
+  <si>
+    <t>Tank commander's independent thermal sight</t>
+  </si>
+  <si>
+    <t>The maximum amount of machine gun on a M1 Abrams is</t>
+  </si>
+  <si>
+    <t>The TUSK packgage for the M1 is designed for</t>
+  </si>
+  <si>
+    <t>Long-range defense against air-to-ground missile attack</t>
+  </si>
+  <si>
+    <t>Short-range defense against chemical and/or biological weapons</t>
+  </si>
+  <si>
+    <t>Short range defense againts infantry-borne AT weapons</t>
+  </si>
+  <si>
+    <t>The maximum achievable speed for the M1 on paved road, while speed governor is installed is:</t>
+  </si>
+  <si>
+    <t>64 km/h</t>
+  </si>
+  <si>
+    <t>72 km/h</t>
+  </si>
+  <si>
+    <t>80 km/h</t>
+  </si>
+  <si>
+    <t>96 km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The upgrade that gives the M60 stabilizer is </t>
+  </si>
+  <si>
+    <t>M60A1</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>RISE</t>
+  </si>
+  <si>
+    <t>M60A2</t>
+  </si>
+  <si>
+    <t>M60A3</t>
+  </si>
+  <si>
+    <t>None, only the M-551 Sheridan can fire this missile</t>
+  </si>
+  <si>
+    <t>Long-range defense against ground-to-ground kinetic projectile e.g APFSDS rounds</t>
+  </si>
+  <si>
+    <t>For the M60A1 update, the carrying capacity of the tank was increased to:</t>
+  </si>
+  <si>
+    <t>60 rounds</t>
+  </si>
+  <si>
+    <t>63 rounds</t>
+  </si>
+  <si>
+    <t>57 rounds</t>
+  </si>
+  <si>
+    <t>61 rounds</t>
+  </si>
+  <si>
+    <t>M48A3</t>
+  </si>
+  <si>
+    <t>M48A5</t>
+  </si>
+  <si>
+    <t>The Magach 6B with the Gal designation means:</t>
+  </si>
+  <si>
+    <t>A new fire control system</t>
+  </si>
+  <si>
+    <t>A new set of passive armor</t>
+  </si>
+  <si>
+    <t>An upgraded engine</t>
+  </si>
+  <si>
+    <t>An upgrade fixing issue with the gun mantlet</t>
+  </si>
+  <si>
+    <t>The Magach 4 is the Israeli name for the tank</t>
+  </si>
+  <si>
+    <t>T-55 tank</t>
+  </si>
+  <si>
+    <t>T-62 tank</t>
+  </si>
+  <si>
+    <t>M48 tank</t>
+  </si>
+  <si>
+    <t>Centurion tank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Nagmachon APC was converted from the hull of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Achzarit APC was converted from the hull of </t>
+  </si>
+  <si>
+    <t>Troop-carrying compartment</t>
+  </si>
+  <si>
+    <t>What are the unique features of a Merkava tank comparing to contemporary Western MBTs?</t>
+  </si>
+  <si>
+    <t>Autoloader</t>
+  </si>
+  <si>
+    <t>Engine located at the front hull</t>
+  </si>
+  <si>
+    <t>Remote-controlled mortar</t>
+  </si>
+  <si>
+    <t>1, 2, 4</t>
+  </si>
+  <si>
+    <t>Mark I</t>
+  </si>
+  <si>
+    <t>Mark II</t>
+  </si>
+  <si>
+    <t>Mark III</t>
+  </si>
+  <si>
+    <t>Mark IV</t>
+  </si>
+  <si>
+    <t>MG251</t>
+  </si>
+  <si>
+    <t>MG252</t>
+  </si>
+  <si>
+    <t>MG253</t>
+  </si>
+  <si>
+    <t>MG254</t>
+  </si>
+  <si>
+    <t>Which Mark gave the Merkava a 120mm gun?</t>
+  </si>
+  <si>
+    <t>Which of the following is a valid designator for variant of the Israeli IMI 120mm gun?</t>
+  </si>
+  <si>
+    <t>The M60 gained capability to fire the MGM-51 Shillelagh missile in variant</t>
+  </si>
+  <si>
+    <t>The F-4 Phantom has a variant to launch AGM-88 SEAD missile, which is:</t>
+  </si>
+  <si>
+    <t>F-4E</t>
+  </si>
+  <si>
+    <t>F-4D</t>
+  </si>
+  <si>
+    <t>F-4X</t>
+  </si>
+  <si>
+    <t>F-4G</t>
+  </si>
+  <si>
+    <t>The Su-27 aircraft is the first Soviet aircraft to adapt:</t>
+  </si>
+  <si>
+    <t>The F-16 Fighting Falcon is equipped with a hull cannon of type</t>
+  </si>
+  <si>
+    <t>20mm M-61 Vulcan</t>
+  </si>
+  <si>
+    <t>7.62mm GAU-2/A</t>
+  </si>
+  <si>
+    <t>40mm L-60 Bofors</t>
+  </si>
+  <si>
+    <t>25mm GAU-12/U</t>
+  </si>
+  <si>
+    <t>The maximum firing rate of a M-61 Vulcan cannon is</t>
+  </si>
+  <si>
+    <t>6000 rpm</t>
+  </si>
+  <si>
+    <t>9000 rpm</t>
+  </si>
+  <si>
+    <t>1500 rpm</t>
+  </si>
+  <si>
+    <t>3000 rpm</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>The main rotor of a UH-1 Huey may have how many rotor blades?</t>
+  </si>
+  <si>
+    <t>The most produced variant of the UH-1 is</t>
+  </si>
+  <si>
+    <t>UH-1A</t>
+  </si>
+  <si>
+    <t>UH-1C</t>
+  </si>
+  <si>
+    <t>UH-1H</t>
+  </si>
+  <si>
+    <t>UH-1N</t>
+  </si>
+  <si>
+    <t>The UH-60 Black Hawk can transport how many people (excluding its own crew)</t>
   </si>
 </sst>
 </file>
@@ -853,10 +1204,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1537704</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>932801</xdr:rowOff>
+      <xdr:rowOff>971550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -887,7 +1238,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5972175" y="8458200"/>
-          <a:ext cx="1476375" cy="932801"/>
+          <a:ext cx="1537704" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1302,10 +1653,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1457325</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>999309</xdr:rowOff>
+      <xdr:rowOff>1064623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1336,7 +1687,251 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5972175" y="11972925"/>
-          <a:ext cx="1457325" cy="999309"/>
+          <a:ext cx="1552575" cy="1064623"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3175</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>847725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="Romania loại biên phi đội MiG-21 từ thời Liên Xô - VnExpress">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{751C6FFE-6F37-47DB-9AB0-08D2320E012C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4562475" y="18449925"/>
+          <a:ext cx="1412875" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1542941</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1009650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="undefined">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48EA95F-0ADE-4B76-BCEF-53F96BEC19B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5972175" y="18449925"/>
+          <a:ext cx="1542941" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1501126</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1000125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491BEE7E-01E2-4FAC-8B12-BD1CCD7359A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3057525" y="18449925"/>
+          <a:ext cx="1501126" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1689100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D6B2C3-8545-4354-B0CD-A55AD8AD9439}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7515225" y="18449925"/>
+          <a:ext cx="1689100" cy="1266825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1655,10 +2250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ31"/>
+  <dimension ref="A1:AMJ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,7 +2261,7 @@
     <col min="1" max="1" width="45.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="1"/>
@@ -1676,7 +2271,7 @@
     <col min="11" max="1024" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1707,8 +2302,26 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="66.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +2335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1748,7 +2361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1774,7 +2387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1800,7 +2413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1826,7 +2439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1852,7 +2465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1878,7 +2491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -1904,7 +2517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
@@ -1930,7 +2543,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1953,7 +2566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1976,7 +2589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -2002,7 +2615,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>71</v>
       </c>
@@ -2025,7 +2638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
@@ -2048,16 +2661,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>11</v>
@@ -2068,22 +2681,22 @@
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>11</v>
@@ -2094,19 +2707,19 @@
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F18" s="1">
         <v>3</v>
@@ -2117,19 +2730,19 @@
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="F19" s="1">
         <v>2</v>
@@ -2140,22 +2753,22 @@
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>11</v>
@@ -2166,22 +2779,22 @@
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>11</v>
@@ -2192,14 +2805,14 @@
     </row>
     <row r="22" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>11</v>
@@ -2210,13 +2823,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>78</v>
@@ -2233,7 +2846,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>25</v>
@@ -2242,133 +2855,154 @@
         <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="F24" s="1">
         <v>3</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="F27" s="1">
         <v>4</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="E28" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="F29" s="1">
         <v>2</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>54</v>
@@ -2376,22 +3010,654 @@
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="1">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1">
+        <v>16</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="E37"/>
+      <c r="F37" s="1">
+        <v>3</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>5</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" s="1">
+        <v>4</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="1">
+        <v>4</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F49" s="1">
+        <v>4</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F52" s="1">
+        <v>3</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F54" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F56" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2</v>
+      </c>
+      <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
+        <v>4</v>
+      </c>
+      <c r="E57" s="1">
+        <v>5</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F58" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B59" s="1">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1">
+        <v>13</v>
+      </c>
+      <c r="E59" s="1">
+        <v>14</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: reloading mechanism for data's js script
</commit_message>
<xml_diff>
--- a/manual/sample_with_image.xlsx
+++ b/manual/sample_with_image.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\exam_builder\manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686897A-8A95-4DB9-A502-09E1640DF7EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3A20A-B594-430B-A404-0F4B5EEE574E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="1635" windowWidth="21180" windowHeight="12570" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="318">
   <si>
     <t>question</t>
   </si>
@@ -612,9 +612,6 @@
     <t>Short-range defense against chemical and/or biological weapons</t>
   </si>
   <si>
-    <t>Short range defense againts infantry-borne AT weapons</t>
-  </si>
-  <si>
     <t>The maximum achievable speed for the M1 on paved road, while speed governor is installed is:</t>
   </si>
   <si>
@@ -832,6 +829,156 @@
   </si>
   <si>
     <t>The UH-60 Black Hawk can transport how many people (excluding its own crew)</t>
+  </si>
+  <si>
+    <t>Short range defense against infantry-borne AT weapons</t>
+  </si>
+  <si>
+    <t>The AH-64 Apache has a front mounted chain gun, which is</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>30mm M230E1</t>
+  </si>
+  <si>
+    <t>The AGM-114 Hellfire missile have a thermobaric warhead variant, and such missile is called</t>
+  </si>
+  <si>
+    <t>AGM-114E</t>
+  </si>
+  <si>
+    <t>AGM-144V</t>
+  </si>
+  <si>
+    <t>AGM-144R</t>
+  </si>
+  <si>
+    <t>AGM-144N</t>
+  </si>
+  <si>
+    <t>The AH-64D variant of the Apache helicopter is nicknamed</t>
+  </si>
+  <si>
+    <t>Kiowa</t>
+  </si>
+  <si>
+    <t>Longbow</t>
+  </si>
+  <si>
+    <t>Cobra</t>
+  </si>
+  <si>
+    <t>Viper</t>
+  </si>
+  <si>
+    <t>The largest caliber artillery currently employed by US military is</t>
+  </si>
+  <si>
+    <t>130mm</t>
+  </si>
+  <si>
+    <t>155mm</t>
+  </si>
+  <si>
+    <t>203mm</t>
+  </si>
+  <si>
+    <t>308mm</t>
+  </si>
+  <si>
+    <t>M270 MLRS</t>
+  </si>
+  <si>
+    <t>The largest tracked rocket-launch artillery currently being employed by the US military is</t>
+  </si>
+  <si>
+    <t>M142 HIMARS</t>
+  </si>
+  <si>
+    <t>M1134 Stryker</t>
+  </si>
+  <si>
+    <t>M777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The minimum range for the 9K58 Smerch is </t>
+  </si>
+  <si>
+    <t>20km</t>
+  </si>
+  <si>
+    <t>26km</t>
+  </si>
+  <si>
+    <t>30km</t>
+  </si>
+  <si>
+    <t>36km</t>
+  </si>
+  <si>
+    <t>The largest caliber artillery currently employed by Russian military is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 9K79 Tochka-U has the maximum range of </t>
+  </si>
+  <si>
+    <t>70km</t>
+  </si>
+  <si>
+    <t>98km</t>
+  </si>
+  <si>
+    <t>120km</t>
+  </si>
+  <si>
+    <t>185km</t>
+  </si>
+  <si>
+    <t>Scud-A</t>
+  </si>
+  <si>
+    <t>Scud-B</t>
+  </si>
+  <si>
+    <t>Scud-C</t>
+  </si>
+  <si>
+    <t>Scud-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The latest variant of Scud missile developed by a Soviet institution is </t>
+  </si>
+  <si>
+    <t>The Iskander-M missile currently employed by the Russian army can carry warhead upto</t>
+  </si>
+  <si>
+    <t>700kg</t>
+  </si>
+  <si>
+    <t>400kg</t>
+  </si>
+  <si>
+    <t>500kg</t>
+  </si>
+  <si>
+    <t>600kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 3M54-1 Kalibr cruise missile, when used to attack land target, has a maximum range of </t>
+  </si>
+  <si>
+    <t>2000km</t>
+  </si>
+  <si>
+    <t>2500km</t>
+  </si>
+  <si>
+    <t>3000km</t>
+  </si>
+  <si>
+    <t>3500km</t>
   </si>
 </sst>
 </file>
@@ -2250,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ59"/>
+  <dimension ref="A1:AMJ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2266,7 +2413,7 @@
     <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="1"/>
     <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
     <col min="11" max="1024" width="8.7109375" style="1"/>
   </cols>
@@ -3079,7 +3226,7 @@
     </row>
     <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>159</v>
@@ -3263,13 +3410,13 @@
         <v>193</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>194</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>195</v>
+        <v>268</v>
       </c>
       <c r="F42" s="1">
         <v>4</v>
@@ -3280,19 +3427,19 @@
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="F43" s="1">
         <v>2</v>
@@ -3303,19 +3450,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="F44" s="1">
         <v>4</v>
@@ -3326,19 +3473,19 @@
     </row>
     <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="F45" s="1">
         <v>2</v>
@@ -3349,19 +3496,19 @@
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="F46" s="1">
         <v>3</v>
@@ -3372,19 +3519,19 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F47" s="1">
         <v>2</v>
@@ -3395,19 +3542,19 @@
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
@@ -3418,19 +3565,19 @@
     </row>
     <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="F49" s="1">
         <v>4</v>
@@ -3441,19 +3588,19 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
@@ -3464,22 +3611,22 @@
     </row>
     <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>11</v>
@@ -3490,19 +3637,19 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="F52" s="1">
         <v>3</v>
@@ -3513,19 +3660,19 @@
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>107</v>
@@ -3539,19 +3686,19 @@
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="F54" s="1">
         <v>4</v>
@@ -3559,19 +3706,19 @@
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -3579,19 +3726,19 @@
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="F56" s="1">
         <v>3</v>
@@ -3599,7 +3746,7 @@
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B57" s="1">
         <v>2</v>
@@ -3614,7 +3761,7 @@
         <v>5</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>54</v>
@@ -3622,19 +3769,19 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="F58" s="1">
         <v>3</v>
@@ -3642,7 +3789,7 @@
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B59" s="1">
         <v>10</v>
@@ -3657,6 +3804,226 @@
         <v>14</v>
       </c>
       <c r="F59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F60" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F61" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F66" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F67" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="F68" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F69" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F70" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>